<commit_message>
Update Indianna Population Dataset.xlsx
</commit_message>
<xml_diff>
--- a/Indianna Population Dataset.xlsx
+++ b/Indianna Population Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garobazarbachian/Desktop/NWU/MSDS 460/Requested-Group-Assignment-3-Integer-Programming-Example---Algorithmic-Redistricting-Spring-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{65740297-CE9A-8D4E-9997-097EE68833E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FC536CF6-6A13-134C-A19E-9AF23500F30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>STATS Indiana</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>% White</t>
   </si>
 </sst>
 </file>
@@ -801,8 +804,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -845,7 +849,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -859,50 +863,52 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1234,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A98" sqref="A7:A98"/>
+      <selection activeCell="M83" sqref="M83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,18 +1257,18 @@
     <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1287,8 +1293,11 @@
       <c r="H5" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1297,8 +1306,9 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1324,8 +1334,12 @@
         <f>SUM(B7:G7)</f>
         <v>36068</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="7">
+        <f>B7/H7</f>
+        <v>0.97349451036930246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1351,8 +1365,12 @@
         <f t="shared" ref="H8:H71" si="0">SUM(B8:G8)</f>
         <v>391449</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="7">
+        <f t="shared" ref="I8:I71" si="1">B8/H8</f>
+        <v>0.7849323922145669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1378,8 +1396,12 @@
         <f t="shared" si="0"/>
         <v>83540</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.8662437155853483</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1405,8 +1427,12 @@
         <f t="shared" si="0"/>
         <v>8719</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96215162289253353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1432,8 +1458,12 @@
         <f t="shared" si="0"/>
         <v>11919</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.95712727577816936</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1459,8 +1489,12 @@
         <f t="shared" si="0"/>
         <v>74164</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.90736745590852708</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1486,8 +1520,12 @@
         <f t="shared" si="0"/>
         <v>15570</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96281310211946047</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1513,8 +1551,12 @@
         <f t="shared" si="0"/>
         <v>20555</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96891267331549502</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1540,8 +1582,12 @@
         <f t="shared" si="0"/>
         <v>37540</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="7">
+        <f t="shared" si="1"/>
+        <v>0.9203249866808737</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1567,8 +1613,12 @@
         <f t="shared" si="0"/>
         <v>124237</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.86564389030643041</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1594,8 +1644,12 @@
         <f t="shared" si="0"/>
         <v>26379</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="7">
+        <f t="shared" si="1"/>
+        <v>0.9666022214640434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1621,8 +1675,12 @@
         <f t="shared" si="0"/>
         <v>32843</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96760344670097131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1648,8 +1706,12 @@
         <f t="shared" si="0"/>
         <v>10536</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96735003796507213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1675,8 +1737,12 @@
         <f t="shared" si="0"/>
         <v>33418</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="7">
+        <f t="shared" si="1"/>
+        <v>0.94742354419773778</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1702,8 +1768,12 @@
         <f t="shared" si="0"/>
         <v>51138</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97058938558410579</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1729,8 +1799,12 @@
         <f t="shared" si="0"/>
         <v>26416</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96134918231374922</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1756,8 +1830,12 @@
         <f t="shared" si="0"/>
         <v>43731</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96967826027303283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1783,8 +1861,12 @@
         <f t="shared" si="0"/>
         <v>112031</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="7">
+        <f t="shared" si="1"/>
+        <v>0.88090796297453389</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -1810,8 +1892,12 @@
         <f t="shared" si="0"/>
         <v>43632</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96775302530253027</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -1837,8 +1923,12 @@
         <f t="shared" si="0"/>
         <v>206890</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="7">
+        <f t="shared" si="1"/>
+        <v>0.892938276378752</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -1864,8 +1954,12 @@
         <f t="shared" si="0"/>
         <v>23349</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96376718489014523</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1891,8 +1985,12 @@
         <f t="shared" si="0"/>
         <v>80714</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="7">
+        <f t="shared" si="1"/>
+        <v>0.89876601333102069</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -1918,8 +2016,12 @@
         <f t="shared" si="0"/>
         <v>16574</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96814287438156144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1945,8 +2047,12 @@
         <f t="shared" si="0"/>
         <v>23028</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97511724856696191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -1972,8 +2078,12 @@
         <f t="shared" si="0"/>
         <v>20327</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="7">
+        <f t="shared" si="1"/>
+        <v>0.95951197914104391</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1999,8 +2109,12 @@
         <f t="shared" si="0"/>
         <v>32993</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="7">
+        <f t="shared" si="1"/>
+        <v>0.93741096596247686</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -2026,8 +2140,12 @@
         <f t="shared" si="0"/>
         <v>66022</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="7">
+        <f t="shared" si="1"/>
+        <v>0.87837387537487499</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
@@ -2053,8 +2171,12 @@
         <f t="shared" si="0"/>
         <v>31006</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97474682319551054</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -2080,8 +2202,12 @@
         <f t="shared" si="0"/>
         <v>364921</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="7">
+        <f t="shared" si="1"/>
+        <v>0.84967979370877533</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -2107,8 +2233,12 @@
         <f t="shared" si="0"/>
         <v>83070</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="7">
+        <f t="shared" si="1"/>
+        <v>0.92190923317683882</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -2134,8 +2264,12 @@
         <f t="shared" si="0"/>
         <v>39851</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96592306341120671</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
@@ -2161,8 +2295,12 @@
         <f t="shared" si="0"/>
         <v>182534</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="7">
+        <f t="shared" si="1"/>
+        <v>0.82900719865887995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -2188,8 +2326,12 @@
         <f t="shared" si="0"/>
         <v>48915</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="7">
+        <f t="shared" si="1"/>
+        <v>0.94825718082387811</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -2215,8 +2357,12 @@
         <f t="shared" si="0"/>
         <v>83574</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="7">
+        <f t="shared" si="1"/>
+        <v>0.86730322827673678</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -2242,8 +2388,12 @@
         <f t="shared" si="0"/>
         <v>36834</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96421784221100071</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -2269,8 +2419,12 @@
         <f t="shared" si="0"/>
         <v>46300</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="7">
+        <f t="shared" si="1"/>
+        <v>0.93479481641468687</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
@@ -2296,8 +2450,12 @@
         <f t="shared" si="0"/>
         <v>33281</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96968240137015116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -2323,8 +2481,12 @@
         <f t="shared" si="0"/>
         <v>20198</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97306664026141199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -2350,8 +2512,12 @@
         <f t="shared" si="0"/>
         <v>32946</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="7">
+        <f t="shared" si="1"/>
+        <v>0.94846111819340739</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
@@ -2377,8 +2543,12 @@
         <f t="shared" si="0"/>
         <v>27536</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96786025566531086</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
@@ -2404,8 +2574,12 @@
         <f t="shared" si="0"/>
         <v>165782</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="7">
+        <f t="shared" si="1"/>
+        <v>0.88457733650215342</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
@@ -2431,8 +2605,12 @@
         <f t="shared" si="0"/>
         <v>35789</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" s="7">
+        <f t="shared" si="1"/>
+        <v>0.93847271508005248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -2458,8 +2636,12 @@
         <f t="shared" si="0"/>
         <v>80826</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="7">
+        <f t="shared" si="1"/>
+        <v>0.95125330957860099</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>52</v>
       </c>
@@ -2485,8 +2667,12 @@
         <f t="shared" si="0"/>
         <v>40866</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97917584299907012</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -2512,8 +2698,12 @@
         <f t="shared" si="0"/>
         <v>499689</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" s="7">
+        <f t="shared" si="1"/>
+        <v>0.70933920898799052</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
@@ -2539,8 +2729,12 @@
         <f t="shared" si="0"/>
         <v>111675</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" s="7">
+        <f t="shared" si="1"/>
+        <v>0.84658159838818003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
@@ -2566,8 +2760,12 @@
         <f t="shared" si="0"/>
         <v>45222</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96691875635752511</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
@@ -2593,8 +2791,12 @@
         <f t="shared" si="0"/>
         <v>131744</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" s="7">
+        <f t="shared" si="1"/>
+        <v>0.8791444012630556</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>57</v>
       </c>
@@ -2620,8 +2822,12 @@
         <f t="shared" si="0"/>
         <v>969466</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" s="7">
+        <f t="shared" si="1"/>
+        <v>0.61879942153721734</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -2647,8 +2853,12 @@
         <f t="shared" si="0"/>
         <v>46332</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96244496244496247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
@@ -2674,8 +2884,12 @@
         <f t="shared" si="0"/>
         <v>9803</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97133530551871872</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>60</v>
       </c>
@@ -2701,8 +2915,12 @@
         <f t="shared" si="0"/>
         <v>35674</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" s="7">
+        <f t="shared" si="1"/>
+        <v>0.90993440600997921</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
@@ -2728,8 +2946,12 @@
         <f t="shared" si="0"/>
         <v>139745</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" s="7">
+        <f t="shared" si="1"/>
+        <v>0.85885004830226486</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
@@ -2755,8 +2977,12 @@
         <f t="shared" si="0"/>
         <v>38273</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="7">
+        <f t="shared" si="1"/>
+        <v>0.95879601808063131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
@@ -2782,8 +3008,12 @@
         <f t="shared" si="0"/>
         <v>72236</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96611108034774906</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
@@ -2809,8 +3039,12 @@
         <f t="shared" si="0"/>
         <v>13823</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96180279244737032</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
@@ -2836,8 +3070,12 @@
         <f t="shared" si="0"/>
         <v>47367</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96320222940021538</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
@@ -2863,8 +3101,12 @@
         <f t="shared" si="0"/>
         <v>6114</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97055937193326791</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>67</v>
       </c>
@@ -2890,8 +3132,12 @@
         <f t="shared" si="0"/>
         <v>19623</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="7">
+        <f t="shared" si="1"/>
+        <v>0.9597411201141518</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>68</v>
       </c>
@@ -2917,8 +3163,12 @@
         <f t="shared" si="0"/>
         <v>21482</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96806628805511596</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
@@ -2944,8 +3194,12 @@
         <f t="shared" si="0"/>
         <v>16369</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96004642922597594</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
@@ -2971,8 +3225,12 @@
         <f t="shared" si="0"/>
         <v>19183</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" s="7">
+        <f t="shared" si="1"/>
+        <v>0.94328311525830166</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>71</v>
       </c>
@@ -2998,8 +3256,12 @@
         <f t="shared" si="0"/>
         <v>12168</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="7">
+        <f t="shared" si="1"/>
+        <v>0.97000328731097962</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>72</v>
       </c>
@@ -3025,8 +3287,12 @@
         <f t="shared" si="0"/>
         <v>174791</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="7">
+        <f t="shared" si="1"/>
+        <v>0.91217511199089196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
@@ -3052,8 +3318,12 @@
         <f t="shared" si="0"/>
         <v>25063</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="7">
+        <f t="shared" si="1"/>
+        <v>0.96580616845549216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>74</v>
       </c>
@@ -3076,11 +3346,15 @@
         <v>172</v>
       </c>
       <c r="H72" s="3">
-        <f t="shared" ref="H72:H98" si="1">SUM(B72:G72)</f>
+        <f t="shared" ref="H72:H98" si="2">SUM(B72:G72)</f>
         <v>12485</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" s="7">
+        <f t="shared" ref="I72:I100" si="3">B72/H72</f>
+        <v>0.96323588305967156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>75</v>
       </c>
@@ -3103,11 +3377,15 @@
         <v>624</v>
       </c>
       <c r="H73" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37301</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" s="7">
+        <f t="shared" si="3"/>
+        <v>0.92981421409613685</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>76</v>
       </c>
@@ -3130,11 +3408,15 @@
         <v>352</v>
       </c>
       <c r="H74" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24437</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96619879690633059</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>77</v>
       </c>
@@ -3157,11 +3439,15 @@
         <v>380</v>
       </c>
       <c r="H75" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29087</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96881768487640529</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -3184,11 +3470,15 @@
         <v>208</v>
       </c>
       <c r="H76" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16673</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96803214778384217</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>79</v>
       </c>
@@ -3211,11 +3501,15 @@
         <v>9550</v>
       </c>
       <c r="H77" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>272234</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" s="7">
+        <f t="shared" si="3"/>
+        <v>0.79149922493149272</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>80</v>
       </c>
@@ -3238,11 +3532,15 @@
         <v>295</v>
       </c>
       <c r="H78" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24588</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96660972832275904</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>81</v>
       </c>
@@ -3265,11 +3563,15 @@
         <v>676</v>
       </c>
       <c r="H79" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44991</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" s="7">
+        <f t="shared" si="3"/>
+        <v>0.95401302482718764</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
@@ -3292,11 +3594,15 @@
         <v>261</v>
       </c>
       <c r="H80" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19967</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96934942655381384</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>83</v>
       </c>
@@ -3319,11 +3625,15 @@
         <v>361</v>
       </c>
       <c r="H81" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23258</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96805400292372512</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>84</v>
       </c>
@@ -3346,11 +3656,15 @@
         <v>460</v>
       </c>
       <c r="H82" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34725</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82" s="7">
+        <f t="shared" si="3"/>
+        <v>0.9640028797696184</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>85</v>
       </c>
@@ -3373,11 +3687,15 @@
         <v>291</v>
       </c>
       <c r="H83" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20670</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83" s="7">
+        <f t="shared" si="3"/>
+        <v>0.92723754233188194</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>86</v>
       </c>
@@ -3400,11 +3718,15 @@
         <v>133</v>
       </c>
       <c r="H84" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10006</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96512092744353384</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>87</v>
       </c>
@@ -3427,11 +3749,15 @@
         <v>4755</v>
       </c>
       <c r="H85" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>188717</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I85" s="7">
+        <f t="shared" si="3"/>
+        <v>0.82217818214575267</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>88</v>
       </c>
@@ -3454,11 +3780,15 @@
         <v>236</v>
       </c>
       <c r="H86" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15361</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96146084239307339</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>89</v>
       </c>
@@ -3481,11 +3811,15 @@
         <v>115</v>
       </c>
       <c r="H87" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6952</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87" s="7">
+        <f t="shared" si="3"/>
+        <v>0.9630322209436134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>90</v>
       </c>
@@ -3508,11 +3842,15 @@
         <v>5622</v>
       </c>
       <c r="H88" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>179744</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88" s="7">
+        <f t="shared" si="3"/>
+        <v>0.84495727256542641</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>91</v>
       </c>
@@ -3535,11 +3873,15 @@
         <v>255</v>
       </c>
       <c r="H89" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15451</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96912821176622876</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>92</v>
       </c>
@@ -3562,11 +3904,15 @@
         <v>2824</v>
       </c>
       <c r="H90" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106006</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I90" s="7">
+        <f t="shared" si="3"/>
+        <v>0.87731826500386767</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>93</v>
       </c>
@@ -3589,11 +3935,15 @@
         <v>416</v>
       </c>
       <c r="H91" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30828</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91" s="7">
+        <f t="shared" si="3"/>
+        <v>0.9631828208122486</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>94</v>
       </c>
@@ -3616,11 +3966,15 @@
         <v>98</v>
       </c>
       <c r="H92" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8461</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I92" s="7">
+        <f t="shared" si="3"/>
+        <v>0.97340739865264159</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -3643,11 +3997,15 @@
         <v>1226</v>
       </c>
       <c r="H93" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65185</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I93" s="7">
+        <f t="shared" si="3"/>
+        <v>0.92849581959039651</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -3670,11 +4028,15 @@
         <v>350</v>
       </c>
       <c r="H94" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28224</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94" s="7">
+        <f t="shared" si="3"/>
+        <v>0.97388747165532885</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -3697,11 +4059,15 @@
         <v>2253</v>
       </c>
       <c r="H95" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66273</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I95" s="7">
+        <f t="shared" si="3"/>
+        <v>0.89893320054924331</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>98</v>
       </c>
@@ -3724,11 +4090,15 @@
         <v>403</v>
       </c>
       <c r="H96" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28335</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I96" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96393153343920945</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>99</v>
       </c>
@@ -3751,11 +4121,15 @@
         <v>355</v>
       </c>
       <c r="H97" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24598</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97" s="7">
+        <f t="shared" si="3"/>
+        <v>0.95877713635254902</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>100</v>
       </c>
@@ -3778,28 +4152,42 @@
         <v>553</v>
       </c>
       <c r="H98" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34627</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98" s="7">
+        <f t="shared" si="3"/>
+        <v>0.96722210991422874</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>102</v>
+      </c>
+      <c r="B99" s="3">
+        <f>SUM(B7:B98)</f>
+        <v>5736944</v>
       </c>
       <c r="H99" s="3">
         <f>SUM(H7:H98)</f>
         <v>6833037</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I99" s="7">
+        <f>B99/H99</f>
+        <v>0.83958918998975129</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>101</v>
       </c>
+      <c r="I100" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>

</xml_diff>